<commit_message>
add caffes module and functions list info and delete on it by clainatomi
</commit_message>
<xml_diff>
--- a/documentation/doc.xlsx
+++ b/documentation/doc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Broff\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\api_caffe-orders_git\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -146,12 +146,6 @@
     <t>Caffe</t>
   </si>
   <si>
-    <t>Вернет массив с полями(id, name, addres, phones, working_time, short_info, info, img, album)</t>
-  </si>
-  <si>
-    <t>Вернет многомерный массив кафе с полями(id, name, addres, phones, working_time, short_info, info, img, album)</t>
-  </si>
-  <si>
     <t>Возвращает нужное кафе</t>
   </si>
   <si>
@@ -201,6 +195,12 @@
   </si>
   <si>
     <t xml:space="preserve"> name,  addres,  telephones,  working_time,  short_info,  info,  wifi,  type,  rating,  number_voters,  sum_votes,  preview_img,  album_name </t>
+  </si>
+  <si>
+    <t>Вернет массив с полями(id, name, address, phones, working_time, short_info, info, img, album)</t>
+  </si>
+  <si>
+    <t>Вернет многомерный массив кафе с полями(id, name, address, phones, working_time, short_info, info, img, album)</t>
   </si>
 </sst>
 </file>
@@ -299,12 +299,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -320,9 +314,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -338,9 +338,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -378,7 +378,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -450,7 +450,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,30 +619,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -665,7 +665,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
@@ -686,7 +686,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
@@ -707,20 +707,20 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="9">
+        <v>42</v>
+      </c>
+      <c r="F6" s="7">
         <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -728,7 +728,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
@@ -749,7 +749,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
@@ -770,7 +770,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
@@ -791,7 +791,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
@@ -812,14 +812,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -873,16 +873,16 @@
         <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
@@ -894,76 +894,76 @@
         <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F18" s="2">
         <v>10</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F19" s="2">
         <v>10</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -975,16 +975,16 @@
         <v>32</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F20" s="2">
         <v>10</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>